<commit_message>
add confirm dialog for lasercalc SRMs
</commit_message>
<xml_diff>
--- a/tests/laicpms_stds_tidy.xlsx
+++ b/tests/laicpms_stds_tidy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanlubbers/Desktop/PhD/Keck_lab/Data_reduction/Laser_TRAMp/Current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/jlubbers_usgs_gov/Documents/Research/Coding/laserTRAM-DB/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E85B78E-BD53-D64B-B7C2-AC5B6C40D24C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4E85B78E-BD53-D64B-B7C2-AC5B6C40D24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{258015F2-B947-48A2-AC73-9B9C2817E060}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{76FC7D86-3AF8-6E4F-9A36-EB9464C01D17}"/>
+    <workbookView xWindow="2730" yWindow="1455" windowWidth="21600" windowHeight="11385" xr2:uid="{76FC7D86-3AF8-6E4F-9A36-EB9464C01D17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -949,19 +949,19 @@
   <dimension ref="A1:EU18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BE2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="151" width="10.83203125" style="8"/>
+    <col min="2" max="151" width="10.875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:151" s="1" customFormat="1">
+    <row r="1" spans="1:151" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>151</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:151">
+    <row r="2" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>65</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:151">
+    <row r="3" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>152</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:151">
+    <row r="4" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>153</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:151">
+    <row r="5" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>154</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:151">
+    <row r="6" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>155</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:151">
+    <row r="7" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:151">
+    <row r="8" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>157</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:151">
+    <row r="9" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>158</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:151">
+    <row r="10" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>159</v>
       </c>
@@ -5166,7 +5166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:151">
+    <row r="11" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>160</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:151">
+    <row r="12" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>161</v>
       </c>
@@ -5986,7 +5986,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:151">
+    <row r="13" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>162</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:151">
+    <row r="14" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>163</v>
       </c>
@@ -6827,7 +6827,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:151">
+    <row r="15" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>164</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:151">
+    <row r="16" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>165</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:151">
+    <row r="17" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>166</v>
       </c>
@@ -8099,7 +8099,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="18" spans="1:151">
+    <row r="18" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>167</v>
       </c>

</xml_diff>